<commit_message>
Putting scripts into folders
</commit_message>
<xml_diff>
--- a/Documents/DeckNDungeons_-_Master_Card_List.xlsx
+++ b/Documents/DeckNDungeons_-_Master_Card_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wits\Game Design\Unity Projects\GitHub\DungeonDeckBuilder\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Possum!\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899B3EBD-B7A7-4A78-9A7E-9927CA008AC2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A80946C-E05E-455A-9B09-EBC305B2CE5E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{D548C7A5-E558-4AAD-9C57-0E65F64AFF18}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{D548C7A5-E558-4AAD-9C57-0E65F64AFF18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="328">
   <si>
     <t>Name</t>
   </si>
@@ -751,10 +751,6 @@
     <t>Undying: at the end of a turn shuffle your graveyard and draw one card from it.</t>
   </si>
   <si>
-    <t>add the attack, defence, discard,and burn costs of one card that you discarded this turn to this cards attack. 
-Burn: regain a sigil card from the burnt pile.</t>
-  </si>
-  <si>
     <t>Burn: +2 atk to this card</t>
   </si>
   <si>
@@ -845,10 +841,6 @@
 At the end of an encounter you gain +15 essence.</t>
   </si>
   <si>
-    <t xml:space="preserve">Untapped: gain +1 extra card at the beginning of a turn.
-Undying: draw -1 less card at the end of your turn. </t>
-  </si>
-  <si>
     <t>Comet Fall</t>
   </si>
   <si>
@@ -902,10 +894,6 @@
 On Arrival: shuffle your hand and discard 5 cards.</t>
   </si>
   <si>
-    <t>Action: Gain attack equal to number of cards in your hand.
-Reaction.</t>
-  </si>
-  <si>
     <t>For every 3 cards in the burn pile, ignore 1 card's discard costs this turn.</t>
   </si>
   <si>
@@ -921,10 +909,6 @@
   </si>
   <si>
     <t>Second Wind</t>
-  </si>
-  <si>
-    <t>Burn: Action -Draw your burnt cards attack value into your hand.
-Reaction - Draw your burnt cards defence value from your deck</t>
   </si>
   <si>
     <t>Draw 2 cards</t>
@@ -1027,9 +1011,6 @@
     <t>Core</t>
   </si>
   <si>
-    <t>Each Attack is doubled in strength. If this creature does damage give the player 2 poisons.</t>
-  </si>
-  <si>
     <t>This creature gains +2 attack overall. Every third card burnt from this deck grants 1 
 card draws for this monster if there hand limit is not reached.</t>
   </si>
@@ -1115,6 +1096,33 @@
   </si>
   <si>
     <t>DPS/Enchanter</t>
+  </si>
+  <si>
+    <t>[] L28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw your
+Burn: 
+Action -Draw your burnt card's attack value x2 into your hand.
+Reaction - Draw your burnt card's defence value x2 from the top of your deck </t>
+  </si>
+  <si>
+    <t>Each Attack is doubled in strength. If this creature does damage give the player 2 poisons. If the player's hand is greater than yours draw 1 card.</t>
+  </si>
+  <si>
+    <t>add the attack, defence, and the discard of one card that you discarded this turn to this cards attack. 
+Burn: regain a sigil card from the burnt pile.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Action: Gain attack equal to number of cards in your hand.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Untapped: gain +1 extra card at the beginning of a turn.
+Undying: discard 1 card at the end of your turn. </t>
+  </si>
+  <si>
+    <t>Kindled</t>
   </si>
 </sst>
 </file>
@@ -1303,7 +1311,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1335,6 +1343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -1659,40 +1668,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6480ED20-FAD2-4A05-B9C2-4B59253F9576}">
   <dimension ref="A1:W202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="B75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q93" sqref="Q93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="74.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="93.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="59.6640625" customWidth="1"/>
+    <col min="1" max="1" width="74.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="93.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="40.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>119</v>
       </c>
@@ -1720,8 +1732,11 @@
       <c r="P2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>120</v>
       </c>
@@ -1749,8 +1764,11 @@
       <c r="P3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>121</v>
       </c>
@@ -1778,8 +1796,11 @@
       <c r="P4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>122</v>
       </c>
@@ -1796,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="J5" t="s">
         <v>222</v>
@@ -1807,8 +1828,11 @@
       <c r="P5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>123</v>
       </c>
@@ -1825,7 +1849,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J6" t="s">
         <v>224</v>
@@ -1836,8 +1860,11 @@
       <c r="P6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>124</v>
       </c>
@@ -1854,7 +1881,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>226</v>
+        <v>324</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>224</v>
@@ -1865,13 +1892,16 @@
       <c r="P7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1883,7 +1913,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>276</v>
+        <v>322</v>
       </c>
       <c r="J8" t="s">
         <v>224</v>
@@ -1894,8 +1924,11 @@
       <c r="P8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I9" s="21"/>
       <c r="O9" s="15">
         <v>27</v>
@@ -1903,8 +1936,11 @@
       <c r="P9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Q9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>151</v>
@@ -1923,7 +1959,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>79</v>
       </c>
@@ -1965,6 +2001,9 @@
       <c r="P11" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="Q11" s="23" t="s">
+        <v>327</v>
+      </c>
       <c r="R11" s="1" t="s">
         <v>75</v>
       </c>
@@ -1975,7 +2014,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="6" t="s">
         <v>6</v>
@@ -1997,7 +2036,7 @@
         <v>8</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>222</v>
@@ -2011,6 +2050,12 @@
       <c r="M12" s="3"/>
       <c r="O12">
         <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
       </c>
       <c r="R12">
         <f t="shared" ref="R12:R31" si="0" xml:space="preserve"> $F12*0.5 +$E12</f>
@@ -2020,7 +2065,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="6" t="s">
         <v>11</v>
@@ -2042,7 +2087,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K13" s="3">
         <v>3</v>
@@ -2053,13 +2098,19 @@
       <c r="M13" s="3"/>
       <c r="O13">
         <v>1</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="6" t="s">
         <v>15</v>
@@ -2081,7 +2132,7 @@
         <v>111</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="J14" t="s">
         <v>223</v>
@@ -2096,6 +2147,12 @@
       <c r="O14">
         <v>1</v>
       </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
       <c r="R14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2104,7 +2161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>113</v>
       </c>
@@ -2143,6 +2200,12 @@
       <c r="O15">
         <v>1</v>
       </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
       <c r="R15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2151,13 +2214,13 @@
         <v>90</v>
       </c>
       <c r="V15" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="W15" s="22" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>109</v>
       </c>
@@ -2181,10 +2244,10 @@
         <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K16" s="3">
         <v>2</v>
@@ -2196,6 +2259,12 @@
       <c r="O16">
         <v>1</v>
       </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
       <c r="R16">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2204,7 +2273,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>98</v>
       </c>
@@ -2228,7 +2297,7 @@
         <v>22</v>
       </c>
       <c r="I17" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J17" t="s">
         <v>224</v>
@@ -2243,6 +2312,12 @@
       <c r="O17">
         <v>1</v>
       </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
       <c r="R17">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -2251,7 +2326,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>104</v>
       </c>
@@ -2275,7 +2350,7 @@
         <v>39</v>
       </c>
       <c r="I18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J18" t="s">
         <v>223</v>
@@ -2289,6 +2364,12 @@
       <c r="M18" s="3"/>
       <c r="O18">
         <v>1</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
       </c>
       <c r="R18">
         <f t="shared" si="0"/>
@@ -2298,7 +2379,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>105</v>
       </c>
@@ -2322,7 +2403,7 @@
         <v>41</v>
       </c>
       <c r="I19" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J19" t="s">
         <v>223</v>
@@ -2331,12 +2412,18 @@
         <v>4</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="M19" s="3"/>
       <c r="O19">
         <v>1</v>
       </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
       <c r="R19">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2345,7 +2432,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>110</v>
       </c>
@@ -2372,7 +2459,7 @@
         <v>225</v>
       </c>
       <c r="J20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K20" s="3">
         <v>4</v>
@@ -2383,16 +2470,22 @@
       <c r="M20" s="3"/>
       <c r="O20">
         <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
       </c>
       <c r="R20">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
@@ -2411,10 +2504,10 @@
         <v>27</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K21" s="3">
         <v>3</v>
@@ -2426,6 +2519,12 @@
       <c r="O21">
         <v>1</v>
       </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
       <c r="R21">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2434,7 +2533,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>99</v>
       </c>
@@ -2458,7 +2557,7 @@
         <v>29</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="J22" t="s">
         <v>224</v>
@@ -2472,13 +2571,19 @@
       <c r="M22" s="3"/>
       <c r="O22">
         <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
       </c>
       <c r="R22">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="9" t="s">
         <v>117</v>
@@ -2500,7 +2605,7 @@
         <v>30</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="J23" t="s">
         <v>224</v>
@@ -2514,13 +2619,19 @@
       <c r="M23" s="3"/>
       <c r="O23">
         <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
       </c>
       <c r="R23">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>100</v>
       </c>
@@ -2544,7 +2655,7 @@
         <v>31</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J24" t="s">
         <v>222</v>
@@ -2559,6 +2670,12 @@
       <c r="O24">
         <v>1</v>
       </c>
+      <c r="P24">
+        <v>1</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
       <c r="R24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2567,7 +2684,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -2591,7 +2708,7 @@
         <v>33</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="J25" t="s">
         <v>223</v>
@@ -2605,13 +2722,19 @@
       <c r="M25" s="3"/>
       <c r="O25">
         <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
       </c>
       <c r="R25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>107</v>
       </c>
@@ -2635,10 +2758,10 @@
         <v>47</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>270</v>
+        <v>325</v>
       </c>
       <c r="J26" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K26" s="3">
         <v>4</v>
@@ -2650,6 +2773,12 @@
       <c r="O26">
         <v>1</v>
       </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
       <c r="R26">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2658,7 +2787,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>109</v>
       </c>
@@ -2682,10 +2811,10 @@
         <v>50</v>
       </c>
       <c r="I27" s="22" t="s">
-        <v>254</v>
+        <v>326</v>
       </c>
       <c r="J27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K27" s="3">
         <v>4</v>
@@ -2697,6 +2826,12 @@
       <c r="O27">
         <v>1</v>
       </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
       <c r="R27">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2705,7 +2840,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>102</v>
       </c>
@@ -2729,7 +2864,7 @@
         <v>36</v>
       </c>
       <c r="I28" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="J28" t="s">
         <v>224</v>
@@ -2744,6 +2879,12 @@
       <c r="O28">
         <v>1</v>
       </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>0</v>
+      </c>
       <c r="R28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2752,7 +2893,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>103</v>
       </c>
@@ -2776,7 +2917,7 @@
         <v>26</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J29" t="s">
         <v>224</v>
@@ -2790,6 +2931,12 @@
       <c r="M29" s="3"/>
       <c r="O29">
         <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
       </c>
       <c r="R29">
         <f t="shared" si="0"/>
@@ -2799,7 +2946,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="11" t="s">
         <v>44</v>
@@ -2821,7 +2968,7 @@
         <v>43</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="J30" t="s">
         <v>222</v>
@@ -2835,6 +2982,12 @@
       <c r="M30" s="3"/>
       <c r="O30">
         <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
       </c>
       <c r="R30">
         <f t="shared" si="0"/>
@@ -2844,7 +2997,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>106</v>
       </c>
@@ -2868,7 +3021,7 @@
         <v>45</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="J31" s="20" t="s">
         <v>224</v>
@@ -2882,6 +3035,12 @@
       <c r="M31" s="3"/>
       <c r="O31">
         <v>1</v>
+      </c>
+      <c r="P31">
+        <v>1</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
       </c>
       <c r="R31">
         <f t="shared" si="0"/>
@@ -2891,77 +3050,77 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O32" s="15">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>147</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="J34" s="17"/>
     </row>
-    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>148</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="J35" s="17"/>
       <c r="T35" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>149</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J36" s="17"/>
       <c r="T36" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>150</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="J37" s="17"/>
       <c r="T37" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>146</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="J38" s="17"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I41" s="21"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>139</v>
       </c>
@@ -2989,8 +3148,11 @@
       <c r="P42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>139</v>
       </c>
@@ -3018,13 +3180,16 @@
       <c r="P43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>139</v>
       </c>
       <c r="B44" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -3039,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J44" t="s">
         <v>222</v>
@@ -3050,13 +3215,16 @@
       <c r="P44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>138</v>
       </c>
       <c r="B45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3071,7 +3239,7 @@
         <v>1</v>
       </c>
       <c r="I45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J45" t="s">
         <v>224</v>
@@ -3082,8 +3250,11 @@
       <c r="P45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>138</v>
       </c>
@@ -3103,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J46" t="s">
         <v>223</v>
@@ -3114,8 +3285,11 @@
       <c r="P46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="Q46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>138</v>
       </c>
@@ -3135,7 +3309,7 @@
         <v>3</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J47" t="s">
         <v>222</v>
@@ -3146,8 +3320,11 @@
       <c r="P47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>140</v>
       </c>
@@ -3167,7 +3344,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="22" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J48" t="s">
         <v>224</v>
@@ -3178,8 +3355,11 @@
       <c r="P48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>140</v>
       </c>
@@ -3210,13 +3390,16 @@
       <c r="P49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="Q49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C50" s="21">
         <v>1</v>
@@ -3231,15 +3414,24 @@
         <v>0</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+      <c r="O50" s="21">
+        <v>2</v>
+      </c>
+      <c r="P50" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C51" s="21">
         <v>1</v>
@@ -3254,15 +3446,24 @@
         <v>2</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" s="21" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+      <c r="O51" s="21">
+        <v>2</v>
+      </c>
+      <c r="P51" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C52" s="21">
         <v>0</v>
@@ -3277,15 +3478,24 @@
         <v>-2</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+      <c r="O52" s="21">
+        <v>2</v>
+      </c>
+      <c r="P52" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="21" t="s">
         <v>135</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C53" s="21">
         <v>0</v>
@@ -3300,13 +3510,22 @@
         <v>-2</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K53" s="21" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="54" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O53" s="21">
+        <v>2</v>
+      </c>
+      <c r="P53" s="21">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>135</v>
       </c>
@@ -3326,13 +3545,13 @@
         <v>3</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J54" s="17" t="s">
         <v>224</v>
       </c>
       <c r="K54" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="O54">
         <v>3</v>
@@ -3340,13 +3559,16 @@
       <c r="P54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>135</v>
       </c>
       <c r="B55" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -3361,7 +3583,7 @@
         <v>-3</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="J55" s="17" t="s">
         <v>224</v>
@@ -3373,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O56" s="15">
         <v>58</v>
       </c>
@@ -3381,12 +3603,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>63</v>
       </c>
@@ -3406,7 +3628,7 @@
         <v>64</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J58" t="s">
         <v>224</v>
@@ -3421,7 +3643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>70</v>
       </c>
@@ -3441,7 +3663,7 @@
         <v>64</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J59" t="s">
         <v>224</v>
@@ -3456,7 +3678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>71</v>
       </c>
@@ -3476,7 +3698,7 @@
         <v>64</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J60" t="s">
         <v>224</v>
@@ -3491,7 +3713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>116</v>
       </c>
@@ -3508,7 +3730,7 @@
         <v>-2</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="J61" t="s">
         <v>224</v>
@@ -3517,9 +3739,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -3537,8 +3759,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>74</v>
       </c>
@@ -3547,7 +3769,7 @@
         <v>1.8333333333333333</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>165</v>
       </c>
@@ -3555,7 +3777,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>53</v>
       </c>
@@ -3588,13 +3810,16 @@
       </c>
       <c r="P69">
         <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>2</v>
       </c>
       <c r="R69">
         <f xml:space="preserve"> $F69*0.5 +$E69</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>56</v>
       </c>
@@ -3627,13 +3852,16 @@
       </c>
       <c r="P70">
         <v>2</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
       </c>
       <c r="R70">
         <f xml:space="preserve"> $F70*0.5 +$E70</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="71" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>57</v>
       </c>
@@ -3653,7 +3881,7 @@
         <v>192</v>
       </c>
       <c r="I71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J71" t="s">
         <v>224</v>
@@ -3666,29 +3894,35 @@
       </c>
       <c r="P71">
         <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
       </c>
       <c r="R71">
         <f xml:space="preserve"> $F71*0.5 +$E71</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O72" s="16">
         <v>15</v>
       </c>
       <c r="P72" s="19">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Q72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B73" s="18" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>58</v>
       </c>
@@ -3708,7 +3942,7 @@
         <v>199</v>
       </c>
       <c r="I74" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J74" t="s">
         <v>222</v>
@@ -3720,6 +3954,9 @@
         <v>8</v>
       </c>
       <c r="P74">
+        <v>2</v>
+      </c>
+      <c r="Q74">
         <v>2</v>
       </c>
       <c r="R74">
@@ -3727,7 +3964,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>59</v>
       </c>
@@ -3747,7 +3984,7 @@
         <v>169</v>
       </c>
       <c r="I75" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J75" t="s">
         <v>223</v>
@@ -3760,13 +3997,16 @@
       </c>
       <c r="P75">
         <v>1</v>
+      </c>
+      <c r="Q75">
+        <v>3</v>
       </c>
       <c r="R75">
         <f xml:space="preserve"> $F75*0.5 +$E75</f>
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>60</v>
       </c>
@@ -3786,7 +4026,7 @@
         <v>193</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="J76" t="s">
         <v>222</v>
@@ -3799,13 +4039,16 @@
       </c>
       <c r="P76">
         <v>0</v>
+      </c>
+      <c r="Q76">
+        <v>1</v>
       </c>
       <c r="R76">
         <f xml:space="preserve"> $F76*0.5 +$E76</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>61</v>
       </c>
@@ -3825,7 +4068,7 @@
         <v>198</v>
       </c>
       <c r="I77" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J77" t="s">
         <v>224</v>
@@ -3838,29 +4081,35 @@
       </c>
       <c r="P77">
         <v>1</v>
+      </c>
+      <c r="Q77">
+        <v>0</v>
       </c>
       <c r="R77">
         <f xml:space="preserve"> $F77*0.5 +$E77</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O78" s="15">
         <v>22</v>
       </c>
       <c r="P78" s="19">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Q78">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>173</v>
       </c>
@@ -3880,7 +4129,7 @@
         <v>220</v>
       </c>
       <c r="I80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J80" t="s">
         <v>223</v>
@@ -3894,8 +4143,11 @@
       <c r="P80">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>172</v>
       </c>
@@ -3915,7 +4167,7 @@
         <v>35</v>
       </c>
       <c r="I81" s="17" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="J81" s="17" t="s">
         <v>224</v>
@@ -3929,8 +4181,11 @@
       <c r="P81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>174</v>
       </c>
@@ -3950,7 +4205,7 @@
         <v>35</v>
       </c>
       <c r="I82" s="17" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="J82" s="17" t="s">
         <v>222</v>
@@ -3965,8 +4220,11 @@
       <c r="P82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>175</v>
       </c>
@@ -3986,7 +4244,7 @@
         <v>176</v>
       </c>
       <c r="I83" s="17" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="J83" s="17" t="s">
         <v>224</v>
@@ -4000,8 +4258,11 @@
       <c r="P83">
         <v>2</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>179</v>
       </c>
@@ -4018,10 +4279,10 @@
         <v>3</v>
       </c>
       <c r="H84" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I84" s="17" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="J84" s="17" t="s">
         <v>222</v>
@@ -4035,16 +4296,22 @@
       <c r="P84">
         <v>2</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O85" s="15">
         <v>30</v>
       </c>
       <c r="P85" s="19">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Q85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>188</v>
       </c>
@@ -4052,7 +4319,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>62</v>
       </c>
@@ -4072,7 +4339,7 @@
         <v>191</v>
       </c>
       <c r="I87" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J87" t="s">
         <v>224</v>
@@ -4086,8 +4353,11 @@
       <c r="P87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>65</v>
       </c>
@@ -4104,10 +4374,10 @@
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I88" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J88" t="s">
         <v>223</v>
@@ -4121,8 +4391,11 @@
       <c r="P88">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q88">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>66</v>
       </c>
@@ -4142,7 +4415,7 @@
         <v>191</v>
       </c>
       <c r="I89" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J89" t="s">
         <v>222</v>
@@ -4156,8 +4429,11 @@
       <c r="P89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="Q89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>67</v>
       </c>
@@ -4191,8 +4467,11 @@
       <c r="P90">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>69</v>
       </c>
@@ -4212,7 +4491,7 @@
         <v>63</v>
       </c>
       <c r="I91" s="17" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J91" s="17" t="s">
         <v>223</v>
@@ -4226,11 +4505,14 @@
       <c r="P91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="21"/>
       <c r="B92" s="21" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C92" s="21">
         <v>1</v>
@@ -4249,7 +4531,7 @@
         <v>211</v>
       </c>
       <c r="I92" s="22" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="J92" t="s">
         <v>222</v>
@@ -4263,20 +4545,26 @@
       <c r="P92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O93" s="15">
         <v>45</v>
       </c>
       <c r="P93" s="19">
         <v>15</v>
+      </c>
+      <c r="Q93">
+        <v>10</v>
       </c>
       <c r="R93">
         <f xml:space="preserve"> $F59*0.5 +$E59</f>
         <v>-1.5</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B94" s="1" t="s">
         <v>142</v>
       </c>
@@ -4285,7 +4573,7 @@
         <v>-4.5</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>152</v>
       </c>
@@ -4293,21 +4581,21 @@
         <v>143</v>
       </c>
       <c r="H95" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I95" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H96" s="21" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I96" s="21" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -4315,26 +4603,26 @@
         <v>144</v>
       </c>
       <c r="H97" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="I97" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H98" s="21" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I98" s="21" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B99" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C99"/>
       <c r="D99"/>
@@ -4342,21 +4630,21 @@
       <c r="F99"/>
       <c r="G99"/>
       <c r="H99" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I99" s="17" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="H100" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I100" s="22" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>189</v>
       </c>
@@ -4369,13 +4657,13 @@
       <c r="F101"/>
       <c r="G101"/>
       <c r="H101" t="s">
+        <v>293</v>
+      </c>
+      <c r="I101" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="I101" s="17" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="21"/>
       <c r="B102" s="21"/>
       <c r="C102" s="21"/>
@@ -4384,26 +4672,26 @@
       <c r="F102" s="21"/>
       <c r="G102" s="21"/>
       <c r="H102" s="21" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I102" s="22" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B106" s="18" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>154</v>
       </c>
@@ -4438,7 +4726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>155</v>
       </c>
@@ -4473,7 +4761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>156</v>
       </c>
@@ -4493,7 +4781,7 @@
         <v>192</v>
       </c>
       <c r="I109" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J109" t="s">
         <v>224</v>
@@ -4508,7 +4796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O110" s="15">
         <v>15</v>
       </c>
@@ -4516,7 +4804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>166</v>
       </c>
@@ -4524,7 +4812,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>162</v>
       </c>
@@ -4559,7 +4847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>163</v>
       </c>
@@ -4579,7 +4867,7 @@
         <v>63</v>
       </c>
       <c r="I113" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J113" t="s">
         <v>223</v>
@@ -4594,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>164</v>
       </c>
@@ -4614,7 +4902,7 @@
         <v>63</v>
       </c>
       <c r="I114" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J114" t="s">
         <v>222</v>
@@ -4629,7 +4917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>168</v>
       </c>
@@ -4646,10 +4934,10 @@
         <v>2</v>
       </c>
       <c r="H115" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I115" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J115" t="s">
         <v>223</v>
@@ -4664,7 +4952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O116" s="15">
         <v>22</v>
       </c>
@@ -4672,7 +4960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>187</v>
       </c>
@@ -4680,44 +4968,44 @@
         <v>186</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I118" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I119" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I120" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I121" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I122" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>188</v>
       </c>
@@ -4725,7 +5013,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>205</v>
       </c>
@@ -4745,7 +5033,7 @@
         <v>211</v>
       </c>
       <c r="I125" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L125" t="s">
         <v>201</v>
@@ -4757,7 +5045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>208</v>
       </c>
@@ -4789,7 +5077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>203</v>
       </c>
@@ -4821,7 +5109,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>207</v>
       </c>
@@ -4850,7 +5138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>206</v>
       </c>
@@ -4883,7 +5171,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>204</v>
       </c>
@@ -4916,7 +5204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>217</v>
       </c>
@@ -4942,13 +5230,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>180</v>
       </c>
@@ -4959,7 +5247,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>158</v>
       </c>
@@ -4970,15 +5258,15 @@
         <v>182</v>
       </c>
     </row>
-    <row r="170" spans="15:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="171" spans="15:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="15:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="171" spans="15:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O171" s="15">
         <v>30</v>
       </c>
       <c r="P171" s="19"/>
     </row>
-    <row r="172" spans="15:16" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="15:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>190</v>
       </c>

</xml_diff>